<commit_message>
changed mixed dates format
</commit_message>
<xml_diff>
--- a/r/_data/dates-mixed.xlsx
+++ b/r/_data/dates-mixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncanrager/Desktop/GitHub/code-book/r/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098B925F-565C-034D-B481-3911385CECD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BB21BD-3DD4-D340-82AF-4A522ADEE74E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="14980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5420" yWindow="460" windowWidth="23000" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dates-mixed" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+  <si>
+    <t>grade</t>
+  </si>
   <si>
     <t>class</t>
   </si>
   <si>
-    <t>grade</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
+    <t>9.17.2016</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
@@ -43,9 +46,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>9.17.2016</t>
-  </si>
-  <si>
     <t>7.26.2015</t>
   </si>
   <si>
@@ -56,6 +56,30 @@
   </si>
   <si>
     <t>2.20.2015</t>
+  </si>
+  <si>
+    <t>10 1 16</t>
+  </si>
+  <si>
+    <t>6/7/17</t>
+  </si>
+  <si>
+    <t>6/6/17</t>
+  </si>
+  <si>
+    <t>6/8/17</t>
+  </si>
+  <si>
+    <t>6/9/17</t>
+  </si>
+  <si>
+    <t>6/10/17</t>
+  </si>
+  <si>
+    <t>6/11/17</t>
+  </si>
+  <si>
+    <t>6/12/17</t>
   </si>
 </sst>
 </file>
@@ -541,7 +565,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -899,18 +923,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -921,8 +950,8 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>43015</v>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,85 +961,85 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>42892</v>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>42905</v>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>42242</v>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>42567</v>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>42888</v>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>43116</v>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>42070</v>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,40 +1049,40 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1064,7 +1093,7 @@
       <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1075,63 +1104,63 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" s="1">
-        <v>42892</v>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17" s="1">
-        <v>43020</v>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" s="1">
-        <v>42265</v>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" s="1">
-        <v>42214</v>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" s="1">
-        <v>42241</v>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
-        <v>42640</v>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>